<commit_message>
Add FMEA for Process
</commit_message>
<xml_diff>
--- a/FMEA/FMEA_APP.xlsx
+++ b/FMEA/FMEA_APP.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Strukturerstellung" sheetId="1" r:id="rId1"/>
+    <sheet name="FMEA_APP" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
@@ -1415,245 +1415,245 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2003,685 +2003,692 @@
   <cols>
     <col min="1" max="1" width="14.85546875" customWidth="1"/>
     <col min="2" max="2" width="37.42578125" customWidth="1"/>
-    <col min="3" max="3" width="63.42578125" style="18" customWidth="1"/>
-    <col min="4" max="4" width="35.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.140625" style="15" customWidth="1"/>
-    <col min="6" max="9" width="9.140625" style="18"/>
-    <col min="10" max="10" width="103.140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.42578125" style="16" customWidth="1"/>
+    <col min="4" max="4" width="35.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.140625" style="13" customWidth="1"/>
+    <col min="6" max="9" width="9.140625" style="16"/>
+    <col min="10" max="10" width="103.140625" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="58" t="s">
+      <c r="F1" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="59" t="s">
+      <c r="G1" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="60" t="s">
+      <c r="H1" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="61" t="s">
+      <c r="I1" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="41" t="s">
+      <c r="J1" s="31" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="63"/>
-      <c r="H2" s="64"/>
-      <c r="I2" s="65"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="39"/>
     </row>
     <row r="3" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="61" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="75" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="83" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="E3" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="66">
+      <c r="F3" s="40">
         <v>8</v>
       </c>
-      <c r="G3" s="67">
+      <c r="G3" s="41">
         <v>1</v>
       </c>
-      <c r="H3" s="68">
+      <c r="H3" s="42">
         <v>10</v>
       </c>
-      <c r="I3" s="61">
-        <f>F3*G3*H3</f>
+      <c r="I3" s="35">
+        <f t="shared" ref="I3:I18" si="0">F3*G3*H3</f>
         <v>80</v>
       </c>
-      <c r="J3" s="78" t="s">
+      <c r="J3" s="52" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="21"/>
-      <c r="B4" s="26"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="10" t="s">
+      <c r="A4" s="61"/>
+      <c r="B4" s="76"/>
+      <c r="C4" s="81"/>
+      <c r="D4" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="69">
+      <c r="F4" s="43">
         <v>7</v>
       </c>
-      <c r="G4" s="70">
+      <c r="G4" s="44">
         <v>3</v>
       </c>
-      <c r="H4" s="71">
+      <c r="H4" s="45">
         <v>3</v>
       </c>
-      <c r="I4" s="72">
-        <f>F4*G4*H4</f>
+      <c r="I4" s="46">
+        <f t="shared" si="0"/>
         <v>63</v>
       </c>
-      <c r="J4" s="79" t="s">
+      <c r="J4" s="53" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="21"/>
-      <c r="B5" s="26"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="8" t="s">
+      <c r="A5" s="61"/>
+      <c r="B5" s="76"/>
+      <c r="C5" s="81"/>
+      <c r="D5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="69">
+      <c r="F5" s="43">
         <v>7</v>
       </c>
-      <c r="G5" s="70">
+      <c r="G5" s="44">
         <v>7</v>
       </c>
-      <c r="H5" s="71">
+      <c r="H5" s="45">
         <v>1</v>
       </c>
-      <c r="I5" s="72">
-        <f>F5*G5*H5</f>
+      <c r="I5" s="46">
+        <f t="shared" si="0"/>
         <v>49</v>
       </c>
-      <c r="J5" s="79" t="s">
+      <c r="J5" s="53" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="21"/>
-      <c r="B6" s="27"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="29" t="s">
+      <c r="A6" s="61"/>
+      <c r="B6" s="77"/>
+      <c r="C6" s="82"/>
+      <c r="D6" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="30" t="s">
+      <c r="E6" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="73">
+      <c r="F6" s="47">
         <v>7</v>
       </c>
-      <c r="G6" s="74">
+      <c r="G6" s="48">
         <v>1</v>
       </c>
-      <c r="H6" s="75">
+      <c r="H6" s="49">
         <v>2</v>
       </c>
-      <c r="I6" s="76">
-        <f>F6*G6*H6</f>
+      <c r="I6" s="50">
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="J6" s="80" t="s">
+      <c r="J6" s="54" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="21"/>
-      <c r="B7" s="22" t="s">
+      <c r="A7" s="61"/>
+      <c r="B7" s="75" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="23" t="s">
+      <c r="C7" s="83" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="31" t="s">
+      <c r="D7" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="25" t="s">
+      <c r="E7" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="66">
+      <c r="F7" s="40">
         <v>7</v>
       </c>
-      <c r="G7" s="67">
+      <c r="G7" s="41">
         <v>1</v>
       </c>
-      <c r="H7" s="68">
+      <c r="H7" s="42">
         <v>2</v>
       </c>
-      <c r="I7" s="61">
-        <f>F7*G7*H7</f>
+      <c r="I7" s="35">
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="J7" s="78" t="s">
+      <c r="J7" s="52" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="21"/>
-      <c r="B8" s="26"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="8" t="s">
+      <c r="A8" s="61"/>
+      <c r="B8" s="76"/>
+      <c r="C8" s="81"/>
+      <c r="D8" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="19" t="s">
+      <c r="E8" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="69">
+      <c r="F8" s="43">
         <v>7</v>
       </c>
-      <c r="G8" s="70">
+      <c r="G8" s="44">
         <v>1</v>
       </c>
-      <c r="H8" s="71">
+      <c r="H8" s="45">
         <v>2</v>
       </c>
-      <c r="I8" s="72">
-        <f>F8*G8*H8</f>
+      <c r="I8" s="46">
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="J8" s="79" t="s">
+      <c r="J8" s="53" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="21"/>
-      <c r="B9" s="27"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="32" t="s">
+      <c r="A9" s="61"/>
+      <c r="B9" s="77"/>
+      <c r="C9" s="82"/>
+      <c r="D9" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="33" t="s">
+      <c r="E9" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="F9" s="73">
+      <c r="F9" s="47">
         <v>7</v>
       </c>
-      <c r="G9" s="74">
+      <c r="G9" s="48">
         <v>1</v>
       </c>
-      <c r="H9" s="75">
+      <c r="H9" s="49">
         <v>2</v>
       </c>
-      <c r="I9" s="76">
-        <f>F9*G9*H9</f>
+      <c r="I9" s="50">
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="J9" s="80" t="s">
+      <c r="J9" s="54" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="21"/>
-      <c r="B10" s="22" t="s">
+      <c r="A10" s="61"/>
+      <c r="B10" s="75" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="34" t="s">
+      <c r="C10" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="40" t="s">
+      <c r="D10" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="E10" s="35" t="s">
+      <c r="E10" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="66">
+      <c r="F10" s="40">
         <v>9</v>
       </c>
-      <c r="G10" s="67">
+      <c r="G10" s="41">
         <v>1</v>
       </c>
-      <c r="H10" s="68">
+      <c r="H10" s="42">
         <v>2</v>
       </c>
-      <c r="I10" s="61">
-        <f>F10*G10*H10</f>
+      <c r="I10" s="35">
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="J10" s="78" t="s">
+      <c r="J10" s="52" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="21"/>
-      <c r="B11" s="26"/>
-      <c r="C11" s="4" t="s">
+      <c r="A11" s="61"/>
+      <c r="B11" s="76"/>
+      <c r="C11" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="20" t="s">
+      <c r="E11" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="F11" s="69">
+      <c r="F11" s="43">
         <v>7</v>
       </c>
-      <c r="G11" s="70">
+      <c r="G11" s="44">
         <v>1</v>
       </c>
-      <c r="H11" s="71">
+      <c r="H11" s="45">
         <v>2</v>
       </c>
-      <c r="I11" s="72">
-        <f>F11*G11*H11</f>
+      <c r="I11" s="46">
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="J11" s="79" t="s">
+      <c r="J11" s="53" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="21"/>
-      <c r="B12" s="26"/>
-      <c r="C12" s="4" t="s">
+      <c r="A12" s="61"/>
+      <c r="B12" s="76"/>
+      <c r="C12" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="20" t="s">
+      <c r="E12" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="F12" s="69">
+      <c r="F12" s="43">
         <v>7</v>
       </c>
-      <c r="G12" s="70">
+      <c r="G12" s="44">
         <v>1</v>
       </c>
-      <c r="H12" s="71">
+      <c r="H12" s="45">
         <v>2</v>
       </c>
-      <c r="I12" s="72">
-        <f>F12*G12*H12</f>
+      <c r="I12" s="46">
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="J12" s="79" t="s">
+      <c r="J12" s="53" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="21"/>
-      <c r="B13" s="26"/>
-      <c r="C13" s="3" t="s">
+      <c r="A13" s="61"/>
+      <c r="B13" s="76"/>
+      <c r="C13" s="81" t="s">
         <v>41</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="69">
+      <c r="F13" s="43">
         <v>9</v>
       </c>
-      <c r="G13" s="70">
+      <c r="G13" s="44">
         <v>1</v>
       </c>
-      <c r="H13" s="71">
+      <c r="H13" s="45">
         <v>2</v>
       </c>
-      <c r="I13" s="72">
-        <f>F13*G13*H13</f>
+      <c r="I13" s="46">
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="J13" s="79" t="s">
+      <c r="J13" s="53" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="21"/>
-      <c r="B14" s="27"/>
-      <c r="C14" s="28"/>
-      <c r="D14" s="32" t="s">
+      <c r="A14" s="61"/>
+      <c r="B14" s="77"/>
+      <c r="C14" s="82"/>
+      <c r="D14" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="E14" s="33" t="s">
+      <c r="E14" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="F14" s="73">
+      <c r="F14" s="47">
         <v>7</v>
       </c>
-      <c r="G14" s="74">
+      <c r="G14" s="48">
         <v>1</v>
       </c>
-      <c r="H14" s="75">
+      <c r="H14" s="49">
         <v>2</v>
       </c>
-      <c r="I14" s="76">
-        <f>F14*G14*H14</f>
+      <c r="I14" s="50">
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="J14" s="80" t="s">
+      <c r="J14" s="54" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="21"/>
-      <c r="B15" s="22" t="s">
+      <c r="A15" s="61"/>
+      <c r="B15" s="75" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="34" t="s">
+      <c r="C15" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="D15" s="31" t="s">
+      <c r="D15" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="E15" s="24" t="s">
+      <c r="E15" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="F15" s="66">
+      <c r="F15" s="40">
         <v>9</v>
       </c>
-      <c r="G15" s="67">
+      <c r="G15" s="41">
         <v>1</v>
       </c>
-      <c r="H15" s="68">
+      <c r="H15" s="42">
         <v>2</v>
       </c>
-      <c r="I15" s="61">
-        <f>F15*G15*H15</f>
+      <c r="I15" s="35">
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="J15" s="78" t="s">
+      <c r="J15" s="52" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="21"/>
-      <c r="B16" s="26"/>
-      <c r="C16" s="4" t="s">
+      <c r="A16" s="61"/>
+      <c r="B16" s="76"/>
+      <c r="C16" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="D16" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="E16" s="19" t="s">
+      <c r="E16" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="F16" s="69">
+      <c r="F16" s="43">
         <v>9</v>
       </c>
-      <c r="G16" s="70">
+      <c r="G16" s="44">
         <v>3</v>
       </c>
-      <c r="H16" s="71">
+      <c r="H16" s="45">
         <v>10</v>
       </c>
-      <c r="I16" s="72">
-        <f>F16*G16*H16</f>
+      <c r="I16" s="46">
+        <f t="shared" si="0"/>
         <v>270</v>
       </c>
-      <c r="J16" s="79" t="s">
+      <c r="J16" s="53" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="21"/>
-      <c r="B17" s="27"/>
-      <c r="C17" s="36" t="s">
+      <c r="A17" s="61"/>
+      <c r="B17" s="77"/>
+      <c r="C17" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="D17" s="77" t="s">
+      <c r="D17" s="51" t="s">
         <v>61</v>
       </c>
-      <c r="E17" s="29" t="s">
+      <c r="E17" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="F17" s="73">
+      <c r="F17" s="47">
         <v>7</v>
       </c>
-      <c r="G17" s="74">
+      <c r="G17" s="48">
         <v>1</v>
       </c>
-      <c r="H17" s="75">
+      <c r="H17" s="49">
         <v>2</v>
       </c>
-      <c r="I17" s="76">
-        <f>F17*G17*H17</f>
+      <c r="I17" s="50">
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="J17" s="80"/>
+      <c r="J17" s="54"/>
     </row>
     <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="21"/>
-      <c r="B18" s="22" t="s">
+      <c r="A18" s="61"/>
+      <c r="B18" s="75" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="34" t="s">
+      <c r="C18" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="D18" s="37" t="s">
+      <c r="D18" s="78" t="s">
         <v>28</v>
       </c>
-      <c r="E18" s="37" t="s">
+      <c r="E18" s="78" t="s">
         <v>17</v>
       </c>
-      <c r="F18" s="42">
+      <c r="F18" s="73">
         <v>7</v>
       </c>
-      <c r="G18" s="43">
+      <c r="G18" s="55">
         <v>1</v>
       </c>
-      <c r="H18" s="44">
+      <c r="H18" s="57">
         <v>2</v>
       </c>
-      <c r="I18" s="45">
-        <f>F18*G18*H18</f>
+      <c r="I18" s="59">
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="J18" s="81" t="s">
+      <c r="J18" s="62" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="21"/>
-      <c r="B19" s="26"/>
-      <c r="C19" s="4" t="s">
+      <c r="A19" s="61"/>
+      <c r="B19" s="76"/>
+      <c r="C19" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="46"/>
-      <c r="G19" s="47"/>
-      <c r="H19" s="48"/>
-      <c r="I19" s="49"/>
-      <c r="J19" s="82"/>
+      <c r="D19" s="79"/>
+      <c r="E19" s="79"/>
+      <c r="F19" s="74"/>
+      <c r="G19" s="56"/>
+      <c r="H19" s="58"/>
+      <c r="I19" s="60"/>
+      <c r="J19" s="63"/>
     </row>
     <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="21"/>
-      <c r="B20" s="26"/>
-      <c r="C20" s="4" t="s">
+      <c r="A20" s="61"/>
+      <c r="B20" s="76"/>
+      <c r="C20" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="E20" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="F20" s="69">
+      <c r="F20" s="43">
         <v>7</v>
       </c>
-      <c r="G20" s="70">
+      <c r="G20" s="44">
         <v>1</v>
       </c>
-      <c r="H20" s="71">
+      <c r="H20" s="45">
         <v>2</v>
       </c>
-      <c r="I20" s="72">
+      <c r="I20" s="46">
         <f>F20*G20*H20</f>
         <v>14</v>
       </c>
-      <c r="J20" s="79" t="s">
+      <c r="J20" s="53" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="21"/>
-      <c r="B21" s="26"/>
-      <c r="C21" s="4" t="s">
+      <c r="A21" s="61"/>
+      <c r="B21" s="76"/>
+      <c r="C21" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D21" s="10" t="s">
+      <c r="D21" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E21" s="10" t="s">
+      <c r="E21" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="F21" s="69">
+      <c r="F21" s="43">
         <v>7</v>
       </c>
-      <c r="G21" s="70">
+      <c r="G21" s="44">
         <v>1</v>
       </c>
-      <c r="H21" s="71">
+      <c r="H21" s="45">
         <v>2</v>
       </c>
-      <c r="I21" s="72">
+      <c r="I21" s="46">
         <f>F21*G21*H21</f>
         <v>14</v>
       </c>
-      <c r="J21" s="79" t="s">
+      <c r="J21" s="53" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="21"/>
-      <c r="B22" s="26"/>
-      <c r="C22" s="17" t="s">
+      <c r="A22" s="61"/>
+      <c r="B22" s="76"/>
+      <c r="C22" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="D22" s="9" t="s">
+      <c r="D22" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="E22" s="10" t="s">
+      <c r="E22" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="F22" s="69">
+      <c r="F22" s="43">
         <v>7</v>
       </c>
-      <c r="G22" s="70">
+      <c r="G22" s="44">
         <v>1</v>
       </c>
-      <c r="H22" s="71">
+      <c r="H22" s="45">
         <v>2</v>
       </c>
-      <c r="I22" s="72">
+      <c r="I22" s="46">
         <f>F22*G22*H22</f>
         <v>14</v>
       </c>
-      <c r="J22" s="79"/>
+      <c r="J22" s="53"/>
     </row>
     <row r="23" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="21"/>
-      <c r="B23" s="26"/>
-      <c r="C23" s="4" t="s">
+      <c r="A23" s="61"/>
+      <c r="B23" s="76"/>
+      <c r="C23" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" s="79" t="s">
         <v>30</v>
       </c>
-      <c r="E23" s="7" t="s">
+      <c r="E23" s="79" t="s">
         <v>17</v>
       </c>
-      <c r="F23" s="50">
+      <c r="F23" s="65">
         <v>9</v>
       </c>
-      <c r="G23" s="51">
+      <c r="G23" s="67">
         <v>1</v>
       </c>
-      <c r="H23" s="52">
+      <c r="H23" s="69">
         <v>2</v>
       </c>
-      <c r="I23" s="53">
+      <c r="I23" s="71">
         <f>F23*G23*H23</f>
         <v>18</v>
       </c>
-      <c r="J23" s="82" t="s">
+      <c r="J23" s="63" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="21"/>
-      <c r="B24" s="27"/>
-      <c r="C24" s="38" t="s">
+      <c r="A24" s="61"/>
+      <c r="B24" s="77"/>
+      <c r="C24" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="D24" s="39"/>
-      <c r="E24" s="39"/>
-      <c r="F24" s="54"/>
-      <c r="G24" s="55"/>
-      <c r="H24" s="56"/>
-      <c r="I24" s="57"/>
-      <c r="J24" s="83"/>
+      <c r="D24" s="80"/>
+      <c r="E24" s="80"/>
+      <c r="F24" s="66"/>
+      <c r="G24" s="68"/>
+      <c r="H24" s="70"/>
+      <c r="I24" s="72"/>
+      <c r="J24" s="64"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="16"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
-      <c r="C26" s="16"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="16"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
-      <c r="C27" s="16"/>
+      <c r="C27" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="C3:C6"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="B10:B14"/>
+    <mergeCell ref="B15:B17"/>
     <mergeCell ref="G18:G19"/>
     <mergeCell ref="H18:H19"/>
     <mergeCell ref="I18:I19"/>
@@ -2698,13 +2705,6 @@
     <mergeCell ref="D23:D24"/>
     <mergeCell ref="C13:C14"/>
     <mergeCell ref="E23:E24"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="C3:C6"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="B10:B14"/>
-    <mergeCell ref="B15:B17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>